<commit_message>
Implemented working demo, bugfixes in execution, storage of instance params in Ignite,
</commit_message>
<xml_diff>
--- a/backend/arena/arena_development.xlsx
+++ b/backend/arena/arena_development.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>create</t>
   </si>
@@ -22,10 +22,22 @@
     <t>python.Array</t>
   </si>
   <si>
+    <t>__len__</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>wow</t>
+  </si>
+  <si>
     <t>Calculator</t>
   </si>
   <si>
     <t>addme</t>
+  </si>
+  <si>
+    <t>A2</t>
   </si>
   <si>
     <t>subme</t>
@@ -36,13 +48,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -78,25 +96,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -403,86 +424,101 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="2">
         <v>2</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>3</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="2">
         <v>5</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="2">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3">
-        <v>2</v>
-      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="3">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
         <v>18</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="3">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2">
         <v>16</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented __len__ for sequence sheets
</commit_message>
<xml_diff>
--- a/backend/arena/arena_development.xlsx
+++ b/backend/arena/arena_development.xlsx
@@ -96,19 +96,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -118,9 +112,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -430,13 +421,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -469,9 +460,9 @@
         <v>3</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
@@ -486,9 +477,9 @@
       <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1"/>
@@ -501,9 +492,9 @@
       <c r="D4" s="2">
         <v>18</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1"/>
@@ -516,9 +507,9 @@
       <c r="D5" s="2">
         <v>16</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Small improvements to execution
</commit_message>
<xml_diff>
--- a/backend/arena/arena_development.xlsx
+++ b/backend/arena/arena_development.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>create</t>
   </si>
@@ -22,7 +22,7 @@
     <t>python.Array</t>
   </si>
   <si>
-    <t>__len__</t>
+    <t>__getitem__</t>
   </si>
   <si>
     <t>A1</t>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>addme</t>
+  </si>
+  <si>
+    <t>A3</t>
   </si>
   <si>
     <t>A2</t>
@@ -96,13 +99,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -421,13 +427,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -452,17 +458,21 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="3">
+        <v>5</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
@@ -489,8 +499,8 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2">
-        <v>18</v>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -499,7 +509,7 @@
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Added create python.Dict support
</commit_message>
<xml_diff>
--- a/backend/arena/arena_development.xlsx
+++ b/backend/arena/arena_development.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>create</t>
   </si>
@@ -22,6 +22,9 @@
     <t>python.Array</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
     <t>__getitem__</t>
   </si>
   <si>
@@ -44,6 +47,18 @@
   </si>
   <si>
     <t>subme</t>
+  </si>
+  <si>
+    <t>python.Dict</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -99,19 +114,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -421,105 +442,148 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="3">
         <v>2</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="3">
         <v>3</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="1">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="4">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5">
+        <v>16</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1">
         <v>3</v>
       </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added support for create python.Complex
</commit_message>
<xml_diff>
--- a/backend/arena/arena_development.xlsx
+++ b/backend/arena/arena_development.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>create</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>subme</t>
+  </si>
+  <si>
+    <t>python.Complex</t>
   </si>
   <si>
     <t>python.Dict</t>
@@ -76,13 +79,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -114,22 +117,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -442,21 +448,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -487,7 +493,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -501,12 +507,12 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="2"/>
+      <c r="G2" s="4"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="I2" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -520,9 +526,9 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="I3" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1"/>
@@ -537,9 +543,9 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="I4" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1"/>
@@ -549,39 +555,58 @@
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="1">
         <v>16</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="I5" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1"/>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="4"/>
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3">
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="H7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="1">
         <v>3</v>
       </c>
     </row>

</xml_diff>